<commit_message>
plato_lops2 and tess overlaps with our catalogue
</commit_message>
<xml_diff>
--- a/results/GAIA__TESS_candidate__matches.xlsx
+++ b/results/GAIA__TESS_candidate__matches.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -32,13 +32,22 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -68,11 +77,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,22 +460,22 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="9" customWidth="1" min="1" max="1"/>
-    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
     <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="16" customWidth="1" min="5" max="5"/>
-    <col width="23" customWidth="1" min="6" max="6"/>
-    <col width="13" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="30" customWidth="1" min="9" max="9"/>
-    <col width="30" customWidth="1" min="10" max="10"/>
-    <col width="29" customWidth="1" min="11" max="11"/>
-    <col width="9" customWidth="1" min="12" max="12"/>
-    <col width="9" customWidth="1" min="13" max="13"/>
-    <col width="35" customWidth="1" min="14" max="14"/>
-    <col width="42" customWidth="1" min="15" max="15"/>
-    <col width="31" customWidth="1" min="16" max="16"/>
+    <col width="37" customWidth="1" min="5" max="5"/>
+    <col width="36" customWidth="1" min="6" max="6"/>
+    <col width="39" customWidth="1" min="7" max="7"/>
+    <col width="34" customWidth="1" min="8" max="8"/>
+    <col width="31" customWidth="1" min="9" max="9"/>
+    <col width="38" customWidth="1" min="10" max="10"/>
+    <col width="42" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="23" customWidth="1" min="13" max="13"/>
+    <col width="41" customWidth="1" min="14" max="14"/>
+    <col width="32" customWidth="1" min="15" max="15"/>
+    <col width="30" customWidth="1" min="16" max="16"/>
     <col width="20" customWidth="1" min="17" max="17"/>
     <col width="22" customWidth="1" min="18" max="18"/>
   </cols>
@@ -470,12 +483,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>toi</t>
+          <t>TESS Object of Interest</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>tid</t>
+          <t>TESS Input Catalog ID</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -490,65 +503,65 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>pl_tranmid</t>
+          <t>Planet Transit Midpoint Value [BJD]</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Orbital Period [days]</t>
+          <t>Planet Orbital Period Value [days]</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>pl_trandurh</t>
+          <t>Planet Transit Duration Value [hours]</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>pl_trandep</t>
+          <t>Planet Transit Depth Value [ppm]</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="2" t="inlineStr">
         <is>
-          <t>Planet Radius [Earth Radius]</t>
+          <t>Planet Radius Value [R_Earth]</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>Insolation Flux [Earth Flux]</t>
+          <t>Planet Insolation Value [Earth flux]</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>Equilibrium Temperature [K]</t>
+          <t>Planet Equilibrium Temperature Value [K]</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>st_tmag</t>
+          <t>TESS Magnitude</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>st_dist</t>
+          <t>Stellar Distance [pc]</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Stellar Effective Temperature [K]</t>
+          <t>Stellar Effective Temperature Value [K]</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Stellar Surface Gravity [log10(cm/s**2)]</t>
+          <t>Stellar log(g) Value [cm/s**2]</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Stellar Radius [Solar Radius]</t>
+          <t>Stellar Radius Value [R_Sun]</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="2" t="inlineStr">
         <is>
           <t>HZ_Detection_Limit</t>
         </is>
@@ -584,7 +597,7 @@
       <c r="H2" t="n">
         <v>384.6733121</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="3" t="n">
         <v>2.0231121</v>
       </c>
       <c r="J2" t="n">
@@ -608,7 +621,7 @@
       <c r="P2" t="n">
         <v>0.963515</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="Q2" s="3" t="n">
         <v>1.058179580845991</v>
       </c>
       <c r="R2" t="n">
@@ -640,7 +653,7 @@
       <c r="H3" t="n">
         <v>217.3994918</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="3" t="n">
         <v>1.5422129</v>
       </c>
       <c r="J3" t="n">
@@ -664,7 +677,7 @@
       <c r="P3" t="n">
         <v>1.02607</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Q3" s="3" t="n">
         <v>1.244933048070707</v>
       </c>
       <c r="R3" t="n">
@@ -696,7 +709,7 @@
       <c r="H4" t="n">
         <v>555.3352929</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="3" t="n">
         <v>2.7050278</v>
       </c>
       <c r="J4" t="n">
@@ -720,7 +733,7 @@
       <c r="P4" t="n">
         <v>1.02607</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="Q4" s="3" t="n">
         <v>1.244933048070707</v>
       </c>
       <c r="R4" t="n">
@@ -749,7 +762,7 @@
       <c r="H5" t="n">
         <v>195.1972939</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="3" t="n">
         <v>1.6208326</v>
       </c>
       <c r="J5" t="n">
@@ -773,7 +786,7 @@
       <c r="P5" t="n">
         <v>1.02607</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Q5" s="3" t="n">
         <v>1.244933048070707</v>
       </c>
       <c r="R5" t="n">
@@ -805,7 +818,7 @@
       <c r="H6" t="n">
         <v>230.9041397</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="3" t="n">
         <v>0.9558514</v>
       </c>
       <c r="J6" t="n">
@@ -829,7 +842,7 @@
       <c r="P6" t="n">
         <v>0.630715</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="Q6" s="3" t="n">
         <v>1.422947157415711</v>
       </c>
       <c r="R6" t="n">
@@ -861,7 +874,7 @@
       <c r="H7" t="n">
         <v>186.7606727</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="3" t="n">
         <v>0.8856846</v>
       </c>
       <c r="J7" t="n">
@@ -885,7 +898,7 @@
       <c r="P7" t="n">
         <v>0.630715</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Q7" s="3" t="n">
         <v>1.422947157415711</v>
       </c>
       <c r="R7" t="n">
@@ -917,7 +930,7 @@
       <c r="H8" t="n">
         <v>190.7947353</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="3" t="n">
         <v>1.0314874</v>
       </c>
       <c r="J8" t="n">
@@ -941,7 +954,7 @@
       <c r="P8" t="n">
         <v>0.630715</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Q8" s="3" t="n">
         <v>1.422947157415711</v>
       </c>
       <c r="R8" t="n">
@@ -973,7 +986,7 @@
       <c r="H9" t="n">
         <v>321</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="3" t="n">
         <v>1.99779</v>
       </c>
       <c r="J9" t="n">
@@ -997,7 +1010,7 @@
       <c r="P9" t="n">
         <v>1.15</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="Q9" s="3" t="n">
         <v>1.616889990960014</v>
       </c>
       <c r="R9" t="n">
@@ -1029,7 +1042,7 @@
       <c r="H10" t="n">
         <v>25854.2144559</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" s="3" t="n">
         <v>13.3010355</v>
       </c>
       <c r="J10" t="n">
@@ -1053,7 +1066,7 @@
       <c r="P10" t="n">
         <v>0.776484</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="Q10" s="3" t="n">
         <v>1.756279763925608</v>
       </c>
       <c r="R10" t="n">
@@ -1085,7 +1098,7 @@
       <c r="H11" t="n">
         <v>1575</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" s="3" t="n">
         <v>3.12194</v>
       </c>
       <c r="J11" t="n">
@@ -1109,7 +1122,7 @@
       <c r="P11" t="n">
         <v>0.71</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="Q11" s="3" t="n">
         <v>1.768355141422782</v>
       </c>
       <c r="R11" t="n">
@@ -1141,7 +1154,7 @@
       <c r="H12" t="n">
         <v>194</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12" s="3" t="n">
         <v>1.00084</v>
       </c>
       <c r="J12" t="n">
@@ -1165,7 +1178,7 @@
       <c r="P12" t="n">
         <v>0.71</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="Q12" s="3" t="n">
         <v>1.768355141422782</v>
       </c>
       <c r="R12" t="n">
@@ -1197,7 +1210,7 @@
       <c r="H13" t="n">
         <v>790</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13" s="3" t="n">
         <v>2.53704</v>
       </c>
       <c r="J13" t="n">
@@ -1221,7 +1234,7 @@
       <c r="P13" t="n">
         <v>0.88</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="Q13" s="3" t="n">
         <v>1.772154586364076</v>
       </c>
       <c r="R13" t="n">
@@ -1253,7 +1266,7 @@
       <c r="H14" t="n">
         <v>137.9312313</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" s="3" t="n">
         <v>0.8814471</v>
       </c>
       <c r="J14" t="n">
@@ -1277,7 +1290,7 @@
       <c r="P14" t="n">
         <v>0.757603</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Q14" s="3" t="n">
         <v>1.909890670031086</v>
       </c>
       <c r="R14" t="n">
@@ -1309,7 +1322,7 @@
       <c r="H15" t="n">
         <v>940</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" s="3" t="n">
         <v>2.4304</v>
       </c>
       <c r="J15" t="n">
@@ -1333,7 +1346,7 @@
       <c r="P15" t="n">
         <v>0.77</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="Q15" s="3" t="n">
         <v>1.953747416139957</v>
       </c>
       <c r="R15" t="n">
@@ -1365,7 +1378,7 @@
       <c r="H16" t="n">
         <v>501.6058242</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16" s="3" t="n">
         <v>2.2881711</v>
       </c>
       <c r="J16" t="n">
@@ -1389,7 +1402,7 @@
       <c r="P16" t="n">
         <v>0.902932</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="Q16" s="3" t="n">
         <v>2.060089842471463</v>
       </c>
       <c r="R16" t="n">
@@ -1421,7 +1434,7 @@
       <c r="H17" t="n">
         <v>799.3817133</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17" s="3" t="n">
         <v>2.5734283</v>
       </c>
       <c r="J17" t="n">
@@ -1445,7 +1458,7 @@
       <c r="P17" t="n">
         <v>0.902932</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="Q17" s="3" t="n">
         <v>2.060089842471463</v>
       </c>
       <c r="R17" t="n">
@@ -1477,7 +1490,7 @@
       <c r="H18" t="n">
         <v>683</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" s="3" t="n">
         <v>1.7005</v>
       </c>
       <c r="J18" t="n">
@@ -1501,7 +1514,7 @@
       <c r="P18" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="Q18" s="3" t="n">
         <v>2.086618763444284</v>
       </c>
       <c r="R18" t="n">
@@ -1533,7 +1546,7 @@
       <c r="H19" t="n">
         <v>865.169438</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19" s="3" t="n">
         <v>2.2407785</v>
       </c>
       <c r="J19" t="n">
@@ -1557,7 +1570,7 @@
       <c r="P19" t="n">
         <v>0.701499</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="Q19" s="3" t="n">
         <v>2.116113831581009</v>
       </c>
       <c r="R19" t="n">
@@ -1589,7 +1602,7 @@
       <c r="H20" t="n">
         <v>914</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" s="3" t="n">
         <v>2.56374</v>
       </c>
       <c r="J20" t="n">
@@ -1613,7 +1626,7 @@
       <c r="P20" t="n">
         <v>0.8</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="Q20" s="3" t="n">
         <v>2.231973848418512</v>
       </c>
       <c r="R20" t="n">
@@ -1645,7 +1658,7 @@
       <c r="H21" t="n">
         <v>274</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" s="3" t="n">
         <v>1.15554</v>
       </c>
       <c r="J21" t="n">
@@ -1669,7 +1682,7 @@
       <c r="P21" t="n">
         <v>0.75</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="Q21" s="3" t="n">
         <v>2.266108314030604</v>
       </c>
       <c r="R21" t="n">
@@ -1701,7 +1714,7 @@
       <c r="H22" t="n">
         <v>169.7218223</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" s="3" t="n">
         <v>0.9704787</v>
       </c>
       <c r="J22" t="n">
@@ -1725,7 +1738,7 @@
       <c r="P22" t="n">
         <v>0.750709</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="Q22" s="3" t="n">
         <v>2.337273193337812</v>
       </c>
       <c r="R22" t="n">
@@ -1757,7 +1770,7 @@
       <c r="H23" t="n">
         <v>708.9461601</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23" s="3" t="n">
         <v>1.9840882</v>
       </c>
       <c r="J23" t="n">
@@ -1781,7 +1794,7 @@
       <c r="P23" t="n">
         <v>0.618173</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="Q23" s="3" t="n">
         <v>2.343640475796769</v>
       </c>
       <c r="R23" t="n">
@@ -1810,7 +1823,7 @@
       <c r="H24" t="n">
         <v>22040</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24" s="3" t="n">
         <v>16.6553</v>
       </c>
       <c r="J24" t="n">
@@ -1834,7 +1847,7 @@
       <c r="P24" t="n">
         <v>1.11</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="Q24" s="3" t="n">
         <v>2.391281741446773</v>
       </c>
       <c r="R24" t="n">
@@ -1866,7 +1879,7 @@
       <c r="H25" t="n">
         <v>601.9566843</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" s="3" t="n">
         <v>1.860295</v>
       </c>
       <c r="J25" t="n">
@@ -1890,7 +1903,7 @@
       <c r="P25" t="n">
         <v>0.739835</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="Q25" s="3" t="n">
         <v>2.496769003128451</v>
       </c>
       <c r="R25" t="n">
@@ -1922,7 +1935,7 @@
       <c r="H26" t="n">
         <v>240</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" s="3" t="n">
         <v>1.20704</v>
       </c>
       <c r="J26" t="n">
@@ -1946,7 +1959,7 @@
       <c r="P26" t="n">
         <v>0.68</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="Q26" s="3" t="n">
         <v>2.520844037452445</v>
       </c>
       <c r="R26" t="n">
@@ -1978,7 +1991,7 @@
       <c r="H27" t="n">
         <v>1144.1789073</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27" s="3" t="n">
         <v>2.5924633</v>
       </c>
       <c r="J27" t="n">
@@ -2002,7 +2015,7 @@
       <c r="P27" t="n">
         <v>0.661076</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="Q27" s="3" t="n">
         <v>2.573431856217872</v>
       </c>
       <c r="R27" t="n">
@@ -2034,7 +2047,7 @@
       <c r="H28" t="n">
         <v>1019</v>
       </c>
-      <c r="I28" t="n">
+      <c r="I28" s="3" t="n">
         <v>2.28729</v>
       </c>
       <c r="J28" t="n">
@@ -2058,7 +2071,7 @@
       <c r="P28" t="n">
         <v>0.66</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="Q28" s="3" t="n">
         <v>2.573431856217872</v>
       </c>
       <c r="R28" t="n">
@@ -2090,7 +2103,7 @@
       <c r="H29" t="n">
         <v>74.807186</v>
       </c>
-      <c r="I29" t="n">
+      <c r="I29" s="3" t="n">
         <v>0.6501353</v>
       </c>
       <c r="J29" t="n">
@@ -2114,7 +2127,7 @@
       <c r="P29" t="n">
         <v>0.74982</v>
       </c>
-      <c r="Q29" t="n">
+      <c r="Q29" s="3" t="n">
         <v>2.608985362147536</v>
       </c>
       <c r="R29" t="n">
@@ -2146,7 +2159,7 @@
       <c r="H30" t="n">
         <v>543.838848</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I30" s="3" t="n">
         <v>1.8245844</v>
       </c>
       <c r="J30" t="n">
@@ -2170,7 +2183,7 @@
       <c r="P30" t="n">
         <v>0.782479</v>
       </c>
-      <c r="Q30" t="n">
+      <c r="Q30" s="3" t="n">
         <v>2.76374786632559</v>
       </c>
       <c r="R30" t="n">
@@ -2199,7 +2212,7 @@
       <c r="H31" t="n">
         <v>886.4838237</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" s="3" t="n">
         <v>2.5398986</v>
       </c>
       <c r="J31" t="n">
@@ -2223,7 +2236,7 @@
       <c r="P31" t="n">
         <v>0.782479</v>
       </c>
-      <c r="Q31" t="n">
+      <c r="Q31" s="3" t="n">
         <v>2.76374786632559</v>
       </c>
       <c r="R31" t="n">
@@ -2255,7 +2268,7 @@
       <c r="H32" t="n">
         <v>1393.3814802</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" s="3" t="n">
         <v>2.6868893</v>
       </c>
       <c r="J32" t="n">
@@ -2279,7 +2292,7 @@
       <c r="P32" t="n">
         <v>0.732115</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="Q32" s="3" t="n">
         <v>2.839885605748058</v>
       </c>
       <c r="R32" t="n">
@@ -2311,7 +2324,7 @@
       <c r="H33" t="n">
         <v>105.5424205</v>
       </c>
-      <c r="I33" t="n">
+      <c r="I33" s="3" t="n">
         <v>1.3473608</v>
       </c>
       <c r="J33" t="n">
@@ -2335,7 +2348,7 @@
       <c r="P33" t="n">
         <v>1.12993</v>
       </c>
-      <c r="Q33" t="n">
+      <c r="Q33" s="3" t="n">
         <v>2.880011854113967</v>
       </c>
       <c r="R33" t="n">
@@ -2367,7 +2380,7 @@
       <c r="H34" t="n">
         <v>154.3008171</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I34" s="3" t="n">
         <v>1.6221344</v>
       </c>
       <c r="J34" t="n">
@@ -2391,7 +2404,7 @@
       <c r="P34" t="n">
         <v>1.12993</v>
       </c>
-      <c r="Q34" t="n">
+      <c r="Q34" s="3" t="n">
         <v>2.880011854113967</v>
       </c>
       <c r="R34" t="n">
@@ -2423,7 +2436,7 @@
       <c r="H35" t="n">
         <v>2509</v>
       </c>
-      <c r="I35" t="n">
+      <c r="I35" s="3" t="n">
         <v>4.36639</v>
       </c>
       <c r="J35" t="n">
@@ -2447,7 +2460,7 @@
       <c r="P35" t="n">
         <v>0.87</v>
       </c>
-      <c r="Q35" t="n">
+      <c r="Q35" s="3" t="n">
         <v>3.075412942076768</v>
       </c>
       <c r="R35" t="n">
@@ -2479,7 +2492,7 @@
       <c r="H36" t="n">
         <v>2078.1425981</v>
       </c>
-      <c r="I36" t="n">
+      <c r="I36" s="3" t="n">
         <v>3.2809492</v>
       </c>
       <c r="J36" t="n">
@@ -2503,7 +2516,7 @@
       <c r="P36" t="n">
         <v>0.7266319999999999</v>
       </c>
-      <c r="Q36" t="n">
+      <c r="Q36" s="3" t="n">
         <v>3.180623248192477</v>
       </c>
       <c r="R36" t="n">
@@ -2535,7 +2548,7 @@
       <c r="H37" t="n">
         <v>291.0399722</v>
       </c>
-      <c r="I37" t="n">
+      <c r="I37" s="3" t="n">
         <v>1.4741529</v>
       </c>
       <c r="J37" t="n">
@@ -2559,7 +2572,7 @@
       <c r="P37" t="n">
         <v>0.7266319999999999</v>
       </c>
-      <c r="Q37" t="n">
+      <c r="Q37" s="3" t="n">
         <v>3.180623248192477</v>
       </c>
       <c r="R37" t="n">
@@ -2591,7 +2604,7 @@
       <c r="H38" t="n">
         <v>308.8285985</v>
       </c>
-      <c r="I38" t="n">
+      <c r="I38" s="3" t="n">
         <v>1.328654</v>
       </c>
       <c r="J38" t="n">
@@ -2615,7 +2628,7 @@
       <c r="P38" t="n">
         <v>0.639371</v>
       </c>
-      <c r="Q38" t="n">
+      <c r="Q38" s="3" t="n">
         <v>3.21466158162215</v>
       </c>
       <c r="R38" t="n">
@@ -2647,7 +2660,7 @@
       <c r="H39" t="n">
         <v>1125.5354645</v>
       </c>
-      <c r="I39" t="n">
+      <c r="I39" s="3" t="n">
         <v>2.6757659</v>
       </c>
       <c r="J39" t="n">
@@ -2671,7 +2684,7 @@
       <c r="P39" t="n">
         <v>0.802633</v>
       </c>
-      <c r="Q39" t="n">
+      <c r="Q39" s="3" t="n">
         <v>3.281657243391717</v>
       </c>
       <c r="R39" t="n">
@@ -2703,7 +2716,7 @@
       <c r="H40" t="n">
         <v>342.1852102</v>
       </c>
-      <c r="I40" t="n">
+      <c r="I40" s="3" t="n">
         <v>1.3134056</v>
       </c>
       <c r="J40" t="n">
@@ -2727,7 +2740,7 @@
       <c r="P40" t="n">
         <v>0.7017099999999999</v>
       </c>
-      <c r="Q40" t="n">
+      <c r="Q40" s="3" t="n">
         <v>3.403379315970769</v>
       </c>
       <c r="R40" t="n">
@@ -2759,7 +2772,7 @@
       <c r="H41" t="n">
         <v>108.5170828</v>
       </c>
-      <c r="I41" t="n">
+      <c r="I41" s="3" t="n">
         <v>1.3159881</v>
       </c>
       <c r="J41" t="n">
@@ -2783,7 +2796,7 @@
       <c r="P41" t="n">
         <v>1.09843</v>
       </c>
-      <c r="Q41" t="n">
+      <c r="Q41" s="3" t="n">
         <v>3.40741529341964</v>
       </c>
       <c r="R41" t="n">
@@ -2815,7 +2828,7 @@
       <c r="H42" t="n">
         <v>24.5834929</v>
       </c>
-      <c r="I42" t="n">
+      <c r="I42" s="3" t="n">
         <v>0.5531037</v>
       </c>
       <c r="J42" t="n">
@@ -2839,7 +2852,7 @@
       <c r="P42" t="n">
         <v>1.09843</v>
       </c>
-      <c r="Q42" t="n">
+      <c r="Q42" s="3" t="n">
         <v>3.40741529341964</v>
       </c>
       <c r="R42" t="n">
@@ -2871,7 +2884,7 @@
       <c r="H43" t="n">
         <v>1140</v>
       </c>
-      <c r="I43" t="n">
+      <c r="I43" s="3" t="n">
         <v>2.64032</v>
       </c>
       <c r="J43" t="n">
@@ -2895,7 +2908,7 @@
       <c r="P43" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q43" t="n">
+      <c r="Q43" s="3" t="n">
         <v>3.425707330003564</v>
       </c>
       <c r="R43" t="n">
@@ -2927,7 +2940,7 @@
       <c r="H44" t="n">
         <v>580</v>
       </c>
-      <c r="I44" t="n">
+      <c r="I44" s="3" t="n">
         <v>1.69257</v>
       </c>
       <c r="J44" t="n">
@@ -2951,7 +2964,7 @@
       <c r="P44" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q44" t="n">
+      <c r="Q44" s="3" t="n">
         <v>3.425707330003564</v>
       </c>
       <c r="R44" t="n">
@@ -2983,7 +2996,7 @@
       <c r="H45" t="n">
         <v>1656</v>
       </c>
-      <c r="I45" t="n">
+      <c r="I45" s="3" t="n">
         <v>2.62025</v>
       </c>
       <c r="J45" t="n">
@@ -3007,7 +3020,7 @@
       <c r="P45" t="n">
         <v>0.63</v>
       </c>
-      <c r="Q45" t="n">
+      <c r="Q45" s="3" t="n">
         <v>3.521787600818508</v>
       </c>
       <c r="R45" t="n">
@@ -3039,7 +3052,7 @@
       <c r="H46" t="n">
         <v>1199</v>
       </c>
-      <c r="I46" t="n">
+      <c r="I46" s="3" t="n">
         <v>1.99787</v>
       </c>
       <c r="J46" t="n">
@@ -3063,7 +3076,7 @@
       <c r="P46" t="n">
         <v>0.63</v>
       </c>
-      <c r="Q46" t="n">
+      <c r="Q46" s="3" t="n">
         <v>3.521787600818508</v>
       </c>
       <c r="R46" t="n">
@@ -3095,7 +3108,7 @@
       <c r="H47" t="n">
         <v>448</v>
       </c>
-      <c r="I47" t="n">
+      <c r="I47" s="3" t="n">
         <v>1.57606</v>
       </c>
       <c r="J47" t="n">
@@ -3119,7 +3132,7 @@
       <c r="P47" t="n">
         <v>0.8</v>
       </c>
-      <c r="Q47" t="n">
+      <c r="Q47" s="3" t="n">
         <v>3.568330244588864</v>
       </c>
       <c r="R47" t="n">
@@ -3151,7 +3164,7 @@
       <c r="H48" t="n">
         <v>122</v>
       </c>
-      <c r="I48" t="n">
+      <c r="I48" s="3" t="n">
         <v>0.808552</v>
       </c>
       <c r="J48" t="n">
@@ -3175,7 +3188,7 @@
       <c r="P48" t="n">
         <v>0.8</v>
       </c>
-      <c r="Q48" t="n">
+      <c r="Q48" s="3" t="n">
         <v>3.568330244588864</v>
       </c>
       <c r="R48" t="n">
@@ -3207,7 +3220,7 @@
       <c r="H49" t="n">
         <v>842</v>
       </c>
-      <c r="I49" t="n">
+      <c r="I49" s="3" t="n">
         <v>2.64301</v>
       </c>
       <c r="J49" t="n">
@@ -3231,7 +3244,7 @@
       <c r="P49" t="n">
         <v>0.93</v>
       </c>
-      <c r="Q49" t="n">
+      <c r="Q49" s="3" t="n">
         <v>3.649745289465404</v>
       </c>
       <c r="R49" t="n">
@@ -3263,7 +3276,7 @@
       <c r="H50" t="n">
         <v>566.2736451</v>
       </c>
-      <c r="I50" t="n">
+      <c r="I50" s="3" t="n">
         <v>2.0671456</v>
       </c>
       <c r="J50" t="n">
@@ -3287,7 +3300,7 @@
       <c r="P50" t="n">
         <v>0.848675</v>
       </c>
-      <c r="Q50" t="n">
+      <c r="Q50" s="3" t="n">
         <v>3.674405832762042</v>
       </c>
       <c r="R50" t="n">
@@ -3319,7 +3332,7 @@
       <c r="H51" t="n">
         <v>398.6310113</v>
       </c>
-      <c r="I51" t="n">
+      <c r="I51" s="3" t="n">
         <v>1.725417</v>
       </c>
       <c r="J51" t="n">
@@ -3343,7 +3356,7 @@
       <c r="P51" t="n">
         <v>0.841842</v>
       </c>
-      <c r="Q51" t="n">
+      <c r="Q51" s="3" t="n">
         <v>3.769031705355568</v>
       </c>
       <c r="R51" t="n">
@@ -3375,7 +3388,7 @@
       <c r="H52" t="n">
         <v>680.1385904</v>
       </c>
-      <c r="I52" t="n">
+      <c r="I52" s="3" t="n">
         <v>2.1954034</v>
       </c>
       <c r="J52" t="n">
@@ -3399,7 +3412,7 @@
       <c r="P52" t="n">
         <v>0.841842</v>
       </c>
-      <c r="Q52" t="n">
+      <c r="Q52" s="3" t="n">
         <v>3.769031705355568</v>
       </c>
       <c r="R52" t="n">
@@ -3431,7 +3444,7 @@
       <c r="H53" t="n">
         <v>262</v>
       </c>
-      <c r="I53" t="n">
+      <c r="I53" s="3" t="n">
         <v>0.986147</v>
       </c>
       <c r="J53" t="n">
@@ -3455,7 +3468,7 @@
       <c r="P53" t="n">
         <v>0.74</v>
       </c>
-      <c r="Q53" t="n">
+      <c r="Q53" s="3" t="n">
         <v>3.8722412377071</v>
       </c>
       <c r="R53" t="n">
@@ -3487,7 +3500,7 @@
       <c r="H54" t="n">
         <v>668</v>
       </c>
-      <c r="I54" t="n">
+      <c r="I54" s="3" t="n">
         <v>1.68645</v>
       </c>
       <c r="J54" t="n">
@@ -3511,7 +3524,7 @@
       <c r="P54" t="n">
         <v>0.63</v>
       </c>
-      <c r="Q54" t="n">
+      <c r="Q54" s="3" t="n">
         <v>3.917080320565909</v>
       </c>
       <c r="R54" t="n">
@@ -3543,7 +3556,7 @@
       <c r="H55" t="n">
         <v>1655.3509066</v>
       </c>
-      <c r="I55" t="n">
+      <c r="I55" s="3" t="n">
         <v>3.4308988</v>
       </c>
       <c r="J55" t="n">
@@ -3567,7 +3580,7 @@
       <c r="P55" t="n">
         <v>0.844852</v>
       </c>
-      <c r="Q55" t="n">
+      <c r="Q55" s="3" t="n">
         <v>3.979865678119569</v>
       </c>
       <c r="R55" t="n">
@@ -3599,7 +3612,7 @@
       <c r="H56" t="n">
         <v>854</v>
       </c>
-      <c r="I56" t="n">
+      <c r="I56" s="3" t="n">
         <v>1.87042</v>
       </c>
       <c r="J56" t="n">
@@ -3623,7 +3636,7 @@
       <c r="P56" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q56" t="n">
+      <c r="Q56" s="3" t="n">
         <v>3.992721170613064</v>
       </c>
       <c r="R56" t="n">
@@ -3655,7 +3668,7 @@
       <c r="H57" t="n">
         <v>671</v>
       </c>
-      <c r="I57" t="n">
+      <c r="I57" s="3" t="n">
         <v>1.60982</v>
       </c>
       <c r="J57" t="n">
@@ -3679,7 +3692,7 @@
       <c r="P57" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q57" t="n">
+      <c r="Q57" s="3" t="n">
         <v>3.992721170613064</v>
       </c>
       <c r="R57" t="n">
@@ -3711,7 +3724,7 @@
       <c r="H58" t="n">
         <v>317</v>
       </c>
-      <c r="I58" t="n">
+      <c r="I58" s="3" t="n">
         <v>1.15643</v>
       </c>
       <c r="J58" t="n">
@@ -3735,7 +3748,7 @@
       <c r="P58" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q58" t="n">
+      <c r="Q58" s="3" t="n">
         <v>3.992721170613064</v>
       </c>
       <c r="R58" t="n">
@@ -3767,7 +3780,7 @@
       <c r="H59" t="n">
         <v>142</v>
       </c>
-      <c r="I59" t="n">
+      <c r="I59" s="3" t="n">
         <v>0.757588</v>
       </c>
       <c r="J59" t="n">
@@ -3791,7 +3804,7 @@
       <c r="P59" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q59" t="n">
+      <c r="Q59" s="3" t="n">
         <v>3.992721170613064</v>
       </c>
       <c r="R59" t="n">
@@ -3823,7 +3836,7 @@
       <c r="H60" t="n">
         <v>217</v>
       </c>
-      <c r="I60" t="n">
+      <c r="I60" s="3" t="n">
         <v>0.969819</v>
       </c>
       <c r="J60" t="n">
@@ -3847,7 +3860,7 @@
       <c r="P60" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="Q60" t="n">
+      <c r="Q60" s="3" t="n">
         <v>3.992721170613064</v>
       </c>
       <c r="R60" t="n">
@@ -3879,7 +3892,7 @@
       <c r="H61" t="n">
         <v>3852.0299874</v>
       </c>
-      <c r="I61" t="n">
+      <c r="I61" s="3" t="n">
         <v>6.1757682</v>
       </c>
       <c r="J61" t="n">
@@ -3903,7 +3916,7 @@
       <c r="P61" t="n">
         <v>0.951985</v>
       </c>
-      <c r="Q61" t="n">
+      <c r="Q61" s="3" t="n">
         <v>4.006602775726686</v>
       </c>
       <c r="R61" t="n">
@@ -3935,7 +3948,7 @@
       <c r="H62" t="n">
         <v>875</v>
       </c>
-      <c r="I62" t="n">
+      <c r="I62" s="3" t="n">
         <v>2.67607</v>
       </c>
       <c r="J62" t="n">
@@ -3959,7 +3972,7 @@
       <c r="P62" t="n">
         <v>0.96</v>
       </c>
-      <c r="Q62" t="n">
+      <c r="Q62" s="3" t="n">
         <v>4.060332463177636</v>
       </c>
       <c r="R62" t="n">
@@ -3991,7 +4004,7 @@
       <c r="H63" t="n">
         <v>960.7539877</v>
       </c>
-      <c r="I63" t="n">
+      <c r="I63" s="3" t="n">
         <v>3.0010426</v>
       </c>
       <c r="J63" t="n">
@@ -4015,7 +4028,7 @@
       <c r="P63" t="n">
         <v>0.962324</v>
       </c>
-      <c r="Q63" t="n">
+      <c r="Q63" s="3" t="n">
         <v>4.060332463177636</v>
       </c>
       <c r="R63" t="n">
@@ -4047,7 +4060,7 @@
       <c r="H64" t="n">
         <v>300</v>
       </c>
-      <c r="I64" t="n">
+      <c r="I64" s="3" t="n">
         <v>2.26316</v>
       </c>
       <c r="J64" t="n">
@@ -4071,7 +4084,7 @@
       <c r="P64" t="n">
         <v>1.33</v>
       </c>
-      <c r="Q64" t="n">
+      <c r="Q64" s="3" t="n">
         <v>4.090376870471276</v>
       </c>
       <c r="R64" t="n">
@@ -4103,7 +4116,7 @@
       <c r="H65" t="n">
         <v>182.9434914</v>
       </c>
-      <c r="I65" t="n">
+      <c r="I65" s="3" t="n">
         <v>1.0903541</v>
       </c>
       <c r="J65" t="n">
@@ -4127,7 +4140,7 @@
       <c r="P65" t="n">
         <v>0.678033</v>
       </c>
-      <c r="Q65" t="n">
+      <c r="Q65" s="3" t="n">
         <v>4.12818079432414</v>
       </c>
       <c r="R65" t="n">
@@ -4159,7 +4172,7 @@
       <c r="H66" t="n">
         <v>445</v>
       </c>
-      <c r="I66" t="n">
+      <c r="I66" s="3" t="n">
         <v>2.12827</v>
       </c>
       <c r="J66" t="n">
@@ -4183,7 +4196,7 @@
       <c r="P66" t="n">
         <v>1.03</v>
       </c>
-      <c r="Q66" t="n">
+      <c r="Q66" s="3" t="n">
         <v>4.161623333076339</v>
       </c>
       <c r="R66" t="n">
@@ -4215,7 +4228,7 @@
       <c r="H67" t="n">
         <v>228</v>
       </c>
-      <c r="I67" t="n">
+      <c r="I67" s="3" t="n">
         <v>1.7202</v>
       </c>
       <c r="J67" t="n">
@@ -4239,7 +4252,7 @@
       <c r="P67" t="n">
         <v>1.13</v>
       </c>
-      <c r="Q67" t="n">
+      <c r="Q67" s="3" t="n">
         <v>4.208501350154981</v>
       </c>
       <c r="R67" t="n">
@@ -4271,7 +4284,7 @@
       <c r="H68" t="n">
         <v>1906.0596245</v>
       </c>
-      <c r="I68" t="n">
+      <c r="I68" s="3" t="n">
         <v>2.9365337</v>
       </c>
       <c r="J68" t="n">
@@ -4295,7 +4308,7 @@
       <c r="P68" t="n">
         <v>0.6750930000000001</v>
       </c>
-      <c r="Q68" t="n">
+      <c r="Q68" s="3" t="n">
         <v>4.31253190430223</v>
       </c>
       <c r="R68" t="n">
@@ -4327,7 +4340,7 @@
       <c r="H69" t="n">
         <v>341.533</v>
       </c>
-      <c r="I69" t="n">
+      <c r="I69" s="3" t="n">
         <v>2.07554</v>
       </c>
       <c r="J69" t="n">
@@ -4351,7 +4364,7 @@
       <c r="P69" t="n">
         <v>1.02</v>
       </c>
-      <c r="Q69" t="n">
+      <c r="Q69" s="3" t="n">
         <v>4.315781758736281</v>
       </c>
       <c r="R69" t="n">
@@ -4383,7 +4396,7 @@
       <c r="H70" t="n">
         <v>844</v>
       </c>
-      <c r="I70" t="n">
+      <c r="I70" s="3" t="n">
         <v>2.12571</v>
       </c>
       <c r="J70" t="n">
@@ -4407,7 +4420,7 @@
       <c r="P70" t="n">
         <v>0.77</v>
       </c>
-      <c r="Q70" t="n">
+      <c r="Q70" s="3" t="n">
         <v>4.318029703234699</v>
       </c>
       <c r="R70" t="n">
@@ -4439,7 +4452,7 @@
       <c r="H71" t="n">
         <v>653.537141</v>
       </c>
-      <c r="I71" t="n">
+      <c r="I71" s="3" t="n">
         <v>1.9015018</v>
       </c>
       <c r="J71" t="n">
@@ -4463,7 +4476,7 @@
       <c r="P71" t="n">
         <v>0.74413</v>
       </c>
-      <c r="Q71" t="n">
+      <c r="Q71" s="3" t="n">
         <v>4.353113514170607</v>
       </c>
       <c r="R71" t="n">
@@ -4495,7 +4508,7 @@
       <c r="H72" t="n">
         <v>1611</v>
       </c>
-      <c r="I72" t="n">
+      <c r="I72" s="3" t="n">
         <v>3.1867</v>
       </c>
       <c r="J72" t="n">
@@ -4519,7 +4532,7 @@
       <c r="P72" t="n">
         <v>0.77</v>
       </c>
-      <c r="Q72" t="n">
+      <c r="Q72" s="3" t="n">
         <v>4.366730157831123</v>
       </c>
       <c r="R72" t="n">
@@ -4551,7 +4564,7 @@
       <c r="H73" t="n">
         <v>17803</v>
       </c>
-      <c r="I73" t="n">
+      <c r="I73" s="3" t="n">
         <v>16.3776</v>
       </c>
       <c r="J73" t="n">
@@ -4575,7 +4588,7 @@
       <c r="P73" t="n">
         <v>1.19</v>
       </c>
-      <c r="Q73" t="n">
+      <c r="Q73" s="3" t="n">
         <v>4.377038819618784</v>
       </c>
       <c r="R73" t="n">
@@ -4607,7 +4620,7 @@
       <c r="H74" t="n">
         <v>1084</v>
       </c>
-      <c r="I74" t="n">
+      <c r="I74" s="3" t="n">
         <v>3.68209</v>
       </c>
       <c r="J74" t="n">
@@ -4631,7 +4644,7 @@
       <c r="P74" t="n">
         <v>0.76</v>
       </c>
-      <c r="Q74" t="n">
+      <c r="Q74" s="3" t="n">
         <v>4.479953862662206</v>
       </c>
       <c r="R74" t="n">
@@ -4663,7 +4676,7 @@
       <c r="H75" t="n">
         <v>1310.6803156</v>
       </c>
-      <c r="I75" t="n">
+      <c r="I75" s="3" t="n">
         <v>2.2761564</v>
       </c>
       <c r="J75" t="n">
@@ -4687,7 +4700,7 @@
       <c r="P75" t="n">
         <v>0.622512</v>
       </c>
-      <c r="Q75" t="n">
+      <c r="Q75" s="3" t="n">
         <v>4.588032766810645</v>
       </c>
       <c r="R75" t="n">
@@ -4719,7 +4732,7 @@
       <c r="H76" t="n">
         <v>193</v>
       </c>
-      <c r="I76" t="n">
+      <c r="I76" s="3" t="n">
         <v>0.930891</v>
       </c>
       <c r="J76" t="n">
@@ -4743,7 +4756,7 @@
       <c r="P76" t="n">
         <v>0.71</v>
       </c>
-      <c r="Q76" t="n">
+      <c r="Q76" s="3" t="n">
         <v>4.794261754598314</v>
       </c>
       <c r="R76" t="n">
@@ -4775,7 +4788,7 @@
       <c r="H77" t="n">
         <v>926.4111032</v>
       </c>
-      <c r="I77" t="n">
+      <c r="I77" s="3" t="n">
         <v>2.1601741</v>
       </c>
       <c r="J77" t="n">
@@ -4799,7 +4812,7 @@
       <c r="P77" t="n">
         <v>0.6634139999999999</v>
       </c>
-      <c r="Q77" t="n">
+      <c r="Q77" s="3" t="n">
         <v>4.802977507666216</v>
       </c>
       <c r="R77" t="n">
@@ -4831,7 +4844,7 @@
       <c r="H78" t="n">
         <v>1376.1395053</v>
       </c>
-      <c r="I78" t="n">
+      <c r="I78" s="3" t="n">
         <v>2.6735992</v>
       </c>
       <c r="J78" t="n">
@@ -4855,7 +4868,7 @@
       <c r="P78" t="n">
         <v>0.7210839999999999</v>
       </c>
-      <c r="Q78" t="n">
+      <c r="Q78" s="3" t="n">
         <v>4.856890565061564</v>
       </c>
       <c r="R78" t="n">
@@ -4887,7 +4900,7 @@
       <c r="H79" t="n">
         <v>465.3854112</v>
       </c>
-      <c r="I79" t="n">
+      <c r="I79" s="3" t="n">
         <v>1.389031</v>
       </c>
       <c r="J79" t="n">
@@ -4911,7 +4924,7 @@
       <c r="P79" t="n">
         <v>0.603336</v>
       </c>
-      <c r="Q79" t="n">
+      <c r="Q79" s="3" t="n">
         <v>5.02924784540017</v>
       </c>
       <c r="R79" t="n">
@@ -4943,7 +4956,7 @@
       <c r="H80" t="n">
         <v>1149.7328034</v>
       </c>
-      <c r="I80" t="n">
+      <c r="I80" s="3" t="n">
         <v>2.3337648</v>
       </c>
       <c r="J80" t="n">
@@ -4967,7 +4980,7 @@
       <c r="P80" t="n">
         <v>0.700727</v>
       </c>
-      <c r="Q80" t="n">
+      <c r="Q80" s="3" t="n">
         <v>5.066808676581831</v>
       </c>
       <c r="R80" t="n">
@@ -4999,7 +5012,7 @@
       <c r="H81" t="n">
         <v>520.4897607</v>
       </c>
-      <c r="I81" t="n">
+      <c r="I81" s="3" t="n">
         <v>2.9033347</v>
       </c>
       <c r="J81" t="n">
@@ -5023,7 +5036,7 @@
       <c r="P81" t="n">
         <v>1.22568</v>
       </c>
-      <c r="Q81" t="n">
+      <c r="Q81" s="3" t="n">
         <v>5.536407362972046</v>
       </c>
       <c r="R81" t="n">
@@ -5055,7 +5068,7 @@
       <c r="H82" t="n">
         <v>1854.2924324</v>
       </c>
-      <c r="I82" t="n">
+      <c r="I82" s="3" t="n">
         <v>2.6845863</v>
       </c>
       <c r="J82" t="n">
@@ -5079,7 +5092,7 @@
       <c r="P82" t="n">
         <v>0.626722</v>
       </c>
-      <c r="Q82" t="n">
+      <c r="Q82" s="3" t="n">
         <v>5.572070940329513</v>
       </c>
       <c r="R82" t="n">
@@ -5111,7 +5124,7 @@
       <c r="H83" t="n">
         <v>1322.2472746</v>
       </c>
-      <c r="I83" t="n">
+      <c r="I83" s="3" t="n">
         <v>2.2115007</v>
       </c>
       <c r="J83" t="n">
@@ -5135,7 +5148,7 @@
       <c r="P83" t="n">
         <v>0.617519</v>
       </c>
-      <c r="Q83" t="n">
+      <c r="Q83" s="3" t="n">
         <v>5.968498212205658</v>
       </c>
       <c r="R83" t="n">
@@ -5167,7 +5180,7 @@
       <c r="H84" t="n">
         <v>540</v>
       </c>
-      <c r="I84" t="n">
+      <c r="I84" s="3" t="n">
         <v>5.59553</v>
       </c>
       <c r="J84" t="n">
@@ -5191,7 +5204,7 @@
       <c r="P84" t="n">
         <v>0.68</v>
       </c>
-      <c r="Q84" t="n">
+      <c r="Q84" s="3" t="n">
         <v>6.453311691204767</v>
       </c>
       <c r="R84" t="n">
@@ -5223,7 +5236,7 @@
       <c r="H85" t="n">
         <v>34536.7848173</v>
       </c>
-      <c r="I85" t="n">
+      <c r="I85" s="3" t="n">
         <v>11.7996868</v>
       </c>
       <c r="J85" t="n">
@@ -5247,7 +5260,7 @@
       <c r="P85" t="n">
         <v>0.636572</v>
       </c>
-      <c r="Q85" t="n">
+      <c r="Q85" s="3" t="n">
         <v>7.581180974499388</v>
       </c>
       <c r="R85" t="n">
@@ -5279,7 +5292,7 @@
       <c r="H86" t="n">
         <v>518.7240999000001</v>
       </c>
-      <c r="I86" t="n">
+      <c r="I86" s="3" t="n">
         <v>1.6802901</v>
       </c>
       <c r="J86" t="n">
@@ -5303,7 +5316,7 @@
       <c r="P86" t="n">
         <v>0.590924</v>
       </c>
-      <c r="Q86" t="n">
+      <c r="Q86" s="3" t="n">
         <v>8.091722393905563</v>
       </c>
       <c r="R86" t="n">
@@ -5335,7 +5348,7 @@
       <c r="H87" t="n">
         <v>232.5621027</v>
       </c>
-      <c r="I87" t="n">
+      <c r="I87" s="3" t="n">
         <v>2.3917735</v>
       </c>
       <c r="J87" t="n">
@@ -5359,7 +5372,7 @@
       <c r="P87" t="n">
         <v>1.2845</v>
       </c>
-      <c r="Q87" t="n">
+      <c r="Q87" s="3" t="n">
         <v>16.45944919601968</v>
       </c>
       <c r="R87" t="n">
@@ -5391,7 +5404,7 @@
       <c r="H88" t="n">
         <v>180</v>
       </c>
-      <c r="I88" t="n">
+      <c r="I88" s="3" t="n">
         <v>1.77141</v>
       </c>
       <c r="J88" t="n">
@@ -5415,7 +5428,7 @@
       <c r="P88" t="n">
         <v>1.28</v>
       </c>
-      <c r="Q88" t="n">
+      <c r="Q88" s="3" t="n">
         <v>16.45944919601968</v>
       </c>
       <c r="R88" t="n">
@@ -5447,7 +5460,7 @@
       <c r="H89" t="n">
         <v>208.629137</v>
       </c>
-      <c r="I89" t="n">
+      <c r="I89" s="3" t="n">
         <v>2.0754665</v>
       </c>
       <c r="J89" t="n">
@@ -5471,7 +5484,7 @@
       <c r="P89" t="n">
         <v>1.2845</v>
       </c>
-      <c r="Q89" t="n">
+      <c r="Q89" s="3" t="n">
         <v>16.45944919601968</v>
       </c>
       <c r="R89" t="n">
@@ -5503,7 +5516,7 @@
       <c r="H90" t="n">
         <v>300.5227138</v>
       </c>
-      <c r="I90" t="n">
+      <c r="I90" s="3" t="n">
         <v>2.8464941</v>
       </c>
       <c r="J90" t="n">
@@ -5527,7 +5540,7 @@
       <c r="P90" t="n">
         <v>1.42717</v>
       </c>
-      <c r="Q90" t="n">
+      <c r="Q90" s="3" t="n">
         <v>31.3192949850797</v>
       </c>
       <c r="R90" t="n">
@@ -5559,7 +5572,7 @@
       <c r="H91" t="n">
         <v>82.7350431</v>
       </c>
-      <c r="I91" t="n">
+      <c r="I91" s="3" t="n">
         <v>1.3337425</v>
       </c>
       <c r="J91" t="n">
@@ -5583,7 +5596,7 @@
       <c r="P91" t="n">
         <v>1.42717</v>
       </c>
-      <c r="Q91" t="n">
+      <c r="Q91" s="3" t="n">
         <v>31.3192949850797</v>
       </c>
       <c r="R91" t="n">
@@ -5615,7 +5628,7 @@
       <c r="H92" t="n">
         <v>384.0441817</v>
       </c>
-      <c r="I92" t="n">
+      <c r="I92" s="3" t="n">
         <v>2.8743721</v>
       </c>
       <c r="J92" t="n">
@@ -5639,7 +5652,7 @@
       <c r="P92" t="n">
         <v>1.40426</v>
       </c>
-      <c r="Q92" t="n">
+      <c r="Q92" s="3" t="n">
         <v>33.76423036948551</v>
       </c>
       <c r="R92" t="n">
@@ -5671,13 +5684,14 @@
       <c r="H93" t="n">
         <v>2725</v>
       </c>
+      <c r="I93" s="3" t="n"/>
       <c r="L93" t="n">
         <v>9.456</v>
       </c>
       <c r="M93" t="n">
         <v>154.124</v>
       </c>
-      <c r="Q93" t="n">
+      <c r="Q93" s="3" t="n">
         <v>187.1954334784244</v>
       </c>
       <c r="R93" t="n">

</xml_diff>

<commit_message>
Many updates due to SIMBAD changes
</commit_message>
<xml_diff>
--- a/results/GAIA__TESS_candidate__matches.xlsx
+++ b/results/GAIA__TESS_candidate__matches.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1011,7 +1011,7 @@
         <v>1.15</v>
       </c>
       <c r="Q9" s="3" t="n">
-        <v>1.616889990960014</v>
+        <v>1.616889990960015</v>
       </c>
       <c r="R9" t="n">
         <v>0.5469902615930315</v>
@@ -2128,7 +2128,7 @@
         <v>0.74982</v>
       </c>
       <c r="Q29" s="3" t="n">
-        <v>2.608985362147536</v>
+        <v>2.608985367019665</v>
       </c>
       <c r="R29" t="n">
         <v>0.2277199720930105</v>
@@ -2245,63 +2245,63 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2443.01</v>
+        <v>6965.01</v>
       </c>
       <c r="B32" t="n">
-        <v>318753380</v>
+        <v>80224448</v>
       </c>
       <c r="C32" t="n">
-        <v>40.179861</v>
+        <v>103.678273</v>
       </c>
       <c r="D32" t="n">
-        <v>1.199676</v>
+        <v>24.245141</v>
       </c>
       <c r="E32" t="n">
-        <v>2459148.098617</v>
+        <v>2459505.193695</v>
       </c>
       <c r="F32" t="n">
-        <v>15.6692322</v>
+        <v>5.9693397</v>
       </c>
       <c r="G32" t="n">
-        <v>4.562853</v>
+        <v>3.441038</v>
       </c>
       <c r="H32" t="n">
-        <v>1393.3814802</v>
+        <v>105.5424205</v>
       </c>
       <c r="I32" s="3" t="n">
-        <v>2.6868893</v>
+        <v>1.3473608</v>
       </c>
       <c r="J32" t="n">
-        <v>13.2931176</v>
+        <v>334.6170929</v>
       </c>
       <c r="K32" t="n">
-        <v>486.9971964</v>
+        <v>1090.8292631</v>
       </c>
       <c r="L32" t="n">
-        <v>8.296900000000001</v>
+        <v>6.3103</v>
       </c>
       <c r="M32" t="n">
-        <v>23.9258</v>
+        <v>31.1664</v>
       </c>
       <c r="N32" t="n">
-        <v>4214.44</v>
+        <v>6007</v>
       </c>
       <c r="O32" t="n">
-        <v>4.52845</v>
+        <v>4.37729</v>
       </c>
       <c r="P32" t="n">
-        <v>0.732115</v>
+        <v>1.12993</v>
       </c>
       <c r="Q32" s="3" t="n">
-        <v>2.839885605748058</v>
+        <v>2.880011854113967</v>
       </c>
       <c r="R32" t="n">
-        <v>0.1818675256571092</v>
+        <v>0.05173693485062012</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>6965.01</v>
+        <v>6965.02</v>
       </c>
       <c r="B33" t="n">
         <v>80224448</v>
@@ -2313,25 +2313,25 @@
         <v>24.245141</v>
       </c>
       <c r="E33" t="n">
-        <v>2459505.193695</v>
+        <v>2459508.008646</v>
       </c>
       <c r="F33" t="n">
-        <v>5.9693397</v>
+        <v>28.0693949</v>
       </c>
       <c r="G33" t="n">
-        <v>3.441038</v>
+        <v>6.0393818</v>
       </c>
       <c r="H33" t="n">
-        <v>105.5424205</v>
+        <v>154.3008171</v>
       </c>
       <c r="I33" s="3" t="n">
-        <v>1.3473608</v>
+        <v>1.6221344</v>
       </c>
       <c r="J33" t="n">
-        <v>334.6170929</v>
+        <v>42.4755605</v>
       </c>
       <c r="K33" t="n">
-        <v>1090.8292631</v>
+        <v>651.1102456</v>
       </c>
       <c r="L33" t="n">
         <v>6.3103</v>
@@ -2357,58 +2357,58 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>6965.02</v>
+        <v>2443.01</v>
       </c>
       <c r="B34" t="n">
-        <v>80224448</v>
+        <v>318753380</v>
       </c>
       <c r="C34" t="n">
-        <v>103.678273</v>
+        <v>40.179861</v>
       </c>
       <c r="D34" t="n">
-        <v>24.245141</v>
+        <v>1.199676</v>
       </c>
       <c r="E34" t="n">
-        <v>2459508.008646</v>
+        <v>2459148.098617</v>
       </c>
       <c r="F34" t="n">
-        <v>28.0693949</v>
+        <v>15.6692322</v>
       </c>
       <c r="G34" t="n">
-        <v>6.0393818</v>
+        <v>4.562853</v>
       </c>
       <c r="H34" t="n">
-        <v>154.3008171</v>
+        <v>1393.3814802</v>
       </c>
       <c r="I34" s="3" t="n">
-        <v>1.6221344</v>
+        <v>2.6868893</v>
       </c>
       <c r="J34" t="n">
-        <v>42.4755605</v>
+        <v>13.2931176</v>
       </c>
       <c r="K34" t="n">
-        <v>651.1102456</v>
+        <v>486.9971964</v>
       </c>
       <c r="L34" t="n">
-        <v>6.3103</v>
+        <v>8.296900000000001</v>
       </c>
       <c r="M34" t="n">
-        <v>31.1664</v>
+        <v>23.9258</v>
       </c>
       <c r="N34" t="n">
-        <v>6007</v>
+        <v>4214.44</v>
       </c>
       <c r="O34" t="n">
-        <v>4.37729</v>
+        <v>4.52845</v>
       </c>
       <c r="P34" t="n">
-        <v>1.12993</v>
+        <v>0.732115</v>
       </c>
       <c r="Q34" s="3" t="n">
-        <v>2.880011854113967</v>
+        <v>2.970022591198855</v>
       </c>
       <c r="R34" t="n">
-        <v>0.05173693485062012</v>
+        <v>0.1818675256571092</v>
       </c>
     </row>
     <row r="35">
@@ -4925,7 +4925,7 @@
         <v>0.603336</v>
       </c>
       <c r="Q79" s="3" t="n">
-        <v>5.02924784540017</v>
+        <v>5.029247845400172</v>
       </c>
       <c r="R79" t="n">
         <v>0.08879781145072711</v>
@@ -4981,7 +4981,7 @@
         <v>0.700727</v>
       </c>
       <c r="Q80" s="3" t="n">
-        <v>5.066808676581831</v>
+        <v>5.06680867658183</v>
       </c>
       <c r="R80" t="n">
         <v>0.02144133406012659</v>
@@ -5653,7 +5653,7 @@
         <v>1.40426</v>
       </c>
       <c r="Q92" s="3" t="n">
-        <v>33.76423036948551</v>
+        <v>33.7642303694855</v>
       </c>
       <c r="R92" t="n">
         <v>0.05602137878216408</v>
@@ -5692,7 +5692,7 @@
         <v>154.124</v>
       </c>
       <c r="Q93" s="3" t="n">
-        <v>187.1954334784244</v>
+        <v>187.1954334784243</v>
       </c>
       <c r="R93" t="n">
         <v>0.0305854259260738</v>

</xml_diff>